<commit_message>
search box + handle large number
</commit_message>
<xml_diff>
--- a/public/assets/download/meritlist.xlsx
+++ b/public/assets/download/meritlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nurul\fyp2\public\assets\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9A1980-3A1E-49CE-B5DA-99FB8E2A8608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76C08DC-63F8-4AA8-BD89-C63FFBE8DF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,13 +93,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,36 +412,37 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>